<commit_message>
Added minor changes to normal cohort excel sheet
</commit_message>
<xml_diff>
--- a/Home/NormalCohortListPerPanel/NormalCohorts.xlsx
+++ b/Home/NormalCohortListPerPanel/NormalCohorts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjamal/Documents/Work/2.scripts/geneCN/Home/NormalCohortListPerPanel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239A10E7-95FE-DD4C-821B-B460136429EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCF4861-9B4B-8840-90F5-D235AC8710D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,9 +207,6 @@
     <t>1806802-RVR-RMH-4384-0013-B</t>
   </si>
   <si>
-    <t>152683-L031</t>
-  </si>
-  <si>
     <t>151127_M02616_0141_000000000-AK5DT</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>154750-L031-B</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +422,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -470,20 +476,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBDD7EE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -762,7 +760,7 @@
   <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -802,7 +800,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="12">
         <v>367</v>
@@ -819,7 +817,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="12">
         <v>335</v>
@@ -836,7 +834,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="12">
         <v>525</v>
@@ -853,7 +851,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="12">
         <v>643</v>
@@ -861,70 +859,70 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E6" s="12">
-        <v>686</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E7" s="12">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="16">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="16">
         <v>861</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="12">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="12">
-        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -975,7 +973,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -992,7 +990,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1009,7 +1007,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1026,7 +1024,7 @@
         <v>22</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1043,7 +1041,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1060,7 +1058,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1077,7 +1075,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1094,7 +1092,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1111,7 +1109,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1128,7 +1126,7 @@
         <v>22</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1145,7 +1143,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1162,7 +1160,7 @@
         <v>22</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1179,7 +1177,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L24" s="1"/>
     </row>
@@ -1197,7 +1195,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1214,7 +1212,7 @@
         <v>22</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1231,7 +1229,7 @@
         <v>22</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1248,7 +1246,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1265,7 +1263,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1282,7 +1280,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1299,7 +1297,7 @@
         <v>22</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1316,7 +1314,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1333,7 +1331,7 @@
         <v>22</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1350,7 +1348,7 @@
         <v>22</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1367,7 +1365,7 @@
         <v>22</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1384,7 +1382,7 @@
         <v>22</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1401,7 +1399,7 @@
         <v>22</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1418,7 +1416,7 @@
         <v>22</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1435,7 +1433,7 @@
         <v>22</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1452,7 +1450,7 @@
         <v>22</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1469,7 +1467,7 @@
         <v>22</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1486,7 +1484,7 @@
         <v>22</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="21">
@@ -1503,7 +1501,7 @@
         <v>22</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
@@ -1522,7 +1520,7 @@
         <v>24</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="14">
         <v>424</v>
@@ -1557,7 +1555,7 @@
     </row>
     <row r="46" spans="1:12" ht="21">
       <c r="A46" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>20</v>
@@ -1579,7 +1577,7 @@
     </row>
     <row r="47" spans="1:12" ht="21">
       <c r="A47" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>20</v>
@@ -1641,7 +1639,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>20</v>
@@ -1661,7 +1659,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>20</v>
@@ -1701,10 +1699,10 @@
         <v>20</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E53" s="14">
         <v>476</v>
@@ -1718,7 +1716,7 @@
         <v>20</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>22</v>
@@ -1741,7 +1739,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D55" s="14" t="s">
         <v>22</v>
@@ -1764,7 +1762,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>22</v>
@@ -1781,19 +1779,19 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -1804,19 +1802,19 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -1827,19 +1825,19 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -1850,19 +1848,19 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G60" s="9"/>
       <c r="H60" s="11"/>
@@ -1873,19 +1871,19 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
@@ -1896,19 +1894,19 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -1919,19 +1917,19 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -1942,19 +1940,19 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G64" s="9"/>
       <c r="H64" s="11"/>
@@ -1965,19 +1963,19 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
@@ -1988,19 +1986,19 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
@@ -2011,19 +2009,19 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
@@ -2034,19 +2032,19 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
@@ -2057,19 +2055,19 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G69" s="9"/>
       <c r="H69" s="11"/>
@@ -2080,19 +2078,19 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
@@ -2103,19 +2101,19 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
@@ -2126,54 +2124,54 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G72" s="4"/>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B74" s="15" t="s">
-        <v>77</v>
-      </c>
       <c r="C74" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>